<commit_message>
Imagens e Checklist atualizados
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PUCRS\ES_Orientada_a_Modelos\T2_ESModelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274FF063-1E7C-44A2-9394-702A13AB1810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD48EAC0-DC0E-412C-A722-CC513FC0773E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4905" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>TODO</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Histórias de usuários possuem três divisões?</t>
   </si>
   <si>
-    <t>Os cenários possuem a cláusula "then"?</t>
-  </si>
-  <si>
     <t>O salário com bônus é calculado nos testes corretamente?</t>
   </si>
   <si>
@@ -52,6 +49,12 @@
   </si>
   <si>
     <t>Histórias de usuário possuem a cláusula "para"?</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Os cenários possuem a cláusula "então"?</t>
   </si>
 </sst>
 </file>
@@ -463,12 +466,12 @@
   <dimension ref="B1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -484,43 +487,57 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C9">

</xml_diff>